<commit_message>
Core - it3- update registoVars Docs - Formulario_gp
</commit_message>
<xml_diff>
--- a/docs/formulario_GP_em_projecto_lapr4.xlsx
+++ b/docs/formulario_GP_em_projecto_lapr4.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Lista de Itens" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -573,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A225" authorId="0">
+    <comment ref="A231" authorId="0">
       <text>
         <r>
           <rPr>
@@ -598,7 +598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A228" authorId="0">
+    <comment ref="A234" authorId="0">
       <text>
         <r>
           <rPr>
@@ -622,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C228" authorId="0">
+    <comment ref="C234" authorId="0">
       <text>
         <r>
           <rPr>
@@ -646,7 +646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D228" authorId="0">
+    <comment ref="D234" authorId="0">
       <text>
         <r>
           <rPr>
@@ -670,7 +670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I228" authorId="0">
+    <comment ref="I234" authorId="0">
       <text>
         <r>
           <rPr>
@@ -699,7 +699,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="351">
   <si>
     <t>Plano de Sprint</t>
   </si>
@@ -1576,6 +1576,228 @@
   <si>
     <t>Calcular valor final</t>
   </si>
+  <si>
+    <t>6.13</t>
+  </si>
+  <si>
+    <t>Identificação das alterações à gramática criada</t>
+  </si>
+  <si>
+    <t>6.14</t>
+  </si>
+  <si>
+    <t>Alteração da gramática para suportar execução de macros</t>
+  </si>
+  <si>
+    <t>6.15</t>
+  </si>
+  <si>
+    <t>6.16</t>
+  </si>
+  <si>
+    <t>Criação de Diagramas</t>
+  </si>
+  <si>
+    <t>Alteração do código para suportar a nova gramática</t>
+  </si>
+  <si>
+    <t>6.17</t>
+  </si>
+  <si>
+    <t>Permitir execução de macros dentro de fórmulas</t>
+  </si>
+  <si>
+    <t>6.18</t>
+  </si>
+  <si>
+    <t>Atribuir resultados de execuções de macros a células ou variáveis</t>
+  </si>
+  <si>
+    <t>Suportar sincronização entre um grupo de células e uma tabela bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deverá ser possível a sincronização entre uma tabela BD e um grupo de área de células. </t>
+  </si>
+  <si>
+    <t>Verificar se está a sincronizar</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>17.2</t>
+  </si>
+  <si>
+    <t>17.3</t>
+  </si>
+  <si>
+    <t>17.4</t>
+  </si>
+  <si>
+    <t>Criar novo item de opção para sincronização</t>
+  </si>
+  <si>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>17.6</t>
+  </si>
+  <si>
+    <t>17.7</t>
+  </si>
+  <si>
+    <t>Incorporar código referente ao grupo de células</t>
+  </si>
+  <si>
+    <t>Incorporar Código referente à tabela</t>
+  </si>
+  <si>
+    <t>Incorporar Código referente à junção da tabela com grupo de células.</t>
+  </si>
+  <si>
+    <t>Exportar/Importar dados para base de dados ficheiros CLS (Hibernate)</t>
+  </si>
+  <si>
+    <t>Exporta/Importa dados para base de dados ficheiros CLS usando Hibernate</t>
+  </si>
+  <si>
+    <t>Dados correctamente exportados/Importados</t>
+  </si>
+  <si>
+    <t>Exportar para ficheiros HTML usando XLST</t>
+  </si>
+  <si>
+    <t>Exporta dados para ficheiros em formato HTML usando XSLT</t>
+  </si>
+  <si>
+    <t>Exportar/Importar dados de base de dados (Hibernate)</t>
+  </si>
+  <si>
+    <t>Desenvolvimento codigo importação/Exportaca</t>
+  </si>
+  <si>
+    <t>Desenvolver aspecto gráfico folha de cálculo em HTML</t>
+  </si>
+  <si>
+    <t>Desenvolver aspecto gráfico folha de cálculo do Workbook</t>
+  </si>
+  <si>
+    <t>Desenvolver dados escritos para ficheiro XSLT</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>18.2</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>18.4</t>
+  </si>
+  <si>
+    <t>18.4.1</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t>19.2</t>
+  </si>
+  <si>
+    <t>19.3</t>
+  </si>
+  <si>
+    <t>19.4</t>
+  </si>
+  <si>
+    <t>19.4.1</t>
+  </si>
+  <si>
+    <t>19.4.2</t>
+  </si>
+  <si>
+    <t>19.4.3</t>
+  </si>
+  <si>
+    <t>Renovar o use case do envio de informação</t>
+  </si>
+  <si>
+    <t>Criar um use case para a procura de partilha na rede</t>
+  </si>
+  <si>
+    <t>Criar diagrama de sequência que represente o método de segurança da partilha</t>
+  </si>
+  <si>
+    <t>Criar diagrama de sequência do pedido de hosts a rede</t>
+  </si>
+  <si>
+    <t>Apresentar a existência da aplicação numa rede</t>
+  </si>
+  <si>
+    <t>Enviar o que uma instância têm a partilhar na rede</t>
+  </si>
+  <si>
+    <t>Procurar por uma instância na rede com uma ou mais partilhas disponíveis</t>
+  </si>
+  <si>
+    <t>Alterar o método de envio de informação</t>
+  </si>
+  <si>
+    <t>Implementação de introdução de password</t>
+  </si>
+  <si>
+    <t>Asseguar a confidencialidade da palavra secreta</t>
+  </si>
+  <si>
+    <t>Conectar a uma partilha na rede, através de uma lista da mesma</t>
+  </si>
+  <si>
+    <t>Assegurar a segurança de uma partilha</t>
+  </si>
+  <si>
+    <t>Necessário saber os hosts que estão disponíveis para partilha, e não é necessário decorar ip</t>
+  </si>
+  <si>
+    <t>conectar a uma partilha desejada na rede</t>
+  </si>
+  <si>
+    <t>Manter a confidencialidade dos dados partilhados e da partilha em si</t>
+  </si>
+  <si>
+    <t>Conectar a partilhas as quais apenas temos acesso ( password )</t>
+  </si>
+  <si>
+    <t>20.1</t>
+  </si>
+  <si>
+    <t>21.1</t>
+  </si>
+  <si>
+    <t>21.2</t>
+  </si>
+  <si>
+    <t>20.2</t>
+  </si>
+  <si>
+    <t>20.3</t>
+  </si>
+  <si>
+    <t>20.4</t>
+  </si>
+  <si>
+    <t>20.5</t>
+  </si>
+  <si>
+    <t>21.3</t>
+  </si>
+  <si>
+    <t>21.4</t>
+  </si>
+  <si>
+    <t>21.5</t>
+  </si>
 </sst>
 </file>
 
@@ -1584,7 +1806,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1675,8 +1897,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1686,6 +1921,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1845,7 +2086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1944,6 +2185,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2022,6 +2273,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2037,7 +2291,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2469,20 +2723,20 @@
       <c r="C22" s="19"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="53"/>
+      <c r="C23" s="57"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="57"/>
     </row>
     <row r="25" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="55"/>
+      <c r="C25" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2510,58 +2764,58 @@
   <sheetData>
     <row r="1" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="58"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="62"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="61"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="64"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
     </row>
     <row r="6" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -2573,10 +2827,10 @@
       <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="8">
         <v>41078</v>
       </c>
@@ -2832,13 +3086,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="9" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2854,50 +3108,50 @@
   <sheetData>
     <row r="1" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="61"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="64"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="68"/>
     </row>
     <row r="6" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -3061,7 +3315,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>16</v>
@@ -3297,83 +3551,171 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="21" t="s">
+    <row r="26" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>17</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E26" s="3">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3">
+        <v>32</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>18</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="E27" s="3">
+        <v>8</v>
+      </c>
+      <c r="F27" s="3">
+        <v>10</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>19</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E28" s="3">
+        <v>8</v>
+      </c>
+      <c r="F28" s="3">
+        <v>30</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>20</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="E29" s="3">
+        <v>6</v>
+      </c>
+      <c r="F29" s="3">
+        <v>25</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>21</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="E30" s="3">
+        <v>7</v>
+      </c>
+      <c r="F30" s="3">
+        <v>19</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="19" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="19" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="22" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="22" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3382,24 +3724,25 @@
     <mergeCell ref="A2:I5"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G29">
-      <formula1>$G$30:$G$33</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G31">
+      <formula1>$G$32:$G$35</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I281"/>
+  <dimension ref="A1:I287"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="C170" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="11" topLeftCell="C213" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F177" sqref="F177"/>
+      <selection pane="bottomRight" activeCell="C216" sqref="C216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,61 +3754,61 @@
   <sheetData>
     <row r="1" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="61"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="61"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="68"/>
     </row>
     <row r="7" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -5080,74 +5423,74 @@
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="66" t="s">
+      <c r="A98" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B98" s="67"/>
-      <c r="C98" s="67"/>
-      <c r="D98" s="67"/>
-      <c r="E98" s="67"/>
-      <c r="F98" s="67"/>
-      <c r="G98" s="67"/>
-      <c r="H98" s="67"/>
-      <c r="I98" s="68"/>
+      <c r="B98" s="71"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="71"/>
+      <c r="E98" s="71"/>
+      <c r="F98" s="71"/>
+      <c r="G98" s="71"/>
+      <c r="H98" s="71"/>
+      <c r="I98" s="72"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="69" t="s">
+      <c r="A99" s="73" t="s">
         <v>247</v>
       </c>
-      <c r="B99" s="70"/>
-      <c r="C99" s="70"/>
-      <c r="D99" s="70"/>
-      <c r="E99" s="70"/>
-      <c r="F99" s="70"/>
-      <c r="G99" s="70"/>
-      <c r="H99" s="70"/>
-      <c r="I99" s="71"/>
+      <c r="B99" s="74"/>
+      <c r="C99" s="74"/>
+      <c r="D99" s="74"/>
+      <c r="E99" s="74"/>
+      <c r="F99" s="74"/>
+      <c r="G99" s="74"/>
+      <c r="H99" s="74"/>
+      <c r="I99" s="75"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="72"/>
-      <c r="B100" s="73"/>
-      <c r="C100" s="73"/>
-      <c r="D100" s="73"/>
-      <c r="E100" s="73"/>
-      <c r="F100" s="73"/>
-      <c r="G100" s="73"/>
-      <c r="H100" s="73"/>
-      <c r="I100" s="74"/>
+      <c r="A100" s="76"/>
+      <c r="B100" s="77"/>
+      <c r="C100" s="77"/>
+      <c r="D100" s="77"/>
+      <c r="E100" s="77"/>
+      <c r="F100" s="77"/>
+      <c r="G100" s="77"/>
+      <c r="H100" s="77"/>
+      <c r="I100" s="78"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="72"/>
-      <c r="B101" s="73"/>
-      <c r="C101" s="73"/>
-      <c r="D101" s="73"/>
-      <c r="E101" s="73"/>
-      <c r="F101" s="73"/>
-      <c r="G101" s="73"/>
-      <c r="H101" s="73"/>
-      <c r="I101" s="74"/>
+      <c r="A101" s="76"/>
+      <c r="B101" s="77"/>
+      <c r="C101" s="77"/>
+      <c r="D101" s="77"/>
+      <c r="E101" s="77"/>
+      <c r="F101" s="77"/>
+      <c r="G101" s="77"/>
+      <c r="H101" s="77"/>
+      <c r="I101" s="78"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="72"/>
-      <c r="B102" s="73"/>
-      <c r="C102" s="73"/>
-      <c r="D102" s="73"/>
-      <c r="E102" s="73"/>
-      <c r="F102" s="73"/>
-      <c r="G102" s="73"/>
-      <c r="H102" s="73"/>
-      <c r="I102" s="74"/>
+      <c r="A102" s="76"/>
+      <c r="B102" s="77"/>
+      <c r="C102" s="77"/>
+      <c r="D102" s="77"/>
+      <c r="E102" s="77"/>
+      <c r="F102" s="77"/>
+      <c r="G102" s="77"/>
+      <c r="H102" s="77"/>
+      <c r="I102" s="78"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="75"/>
-      <c r="B103" s="76"/>
-      <c r="C103" s="76"/>
-      <c r="D103" s="76"/>
-      <c r="E103" s="76"/>
-      <c r="F103" s="76"/>
-      <c r="G103" s="76"/>
-      <c r="H103" s="76"/>
-      <c r="I103" s="77"/>
+      <c r="A103" s="79"/>
+      <c r="B103" s="80"/>
+      <c r="C103" s="80"/>
+      <c r="D103" s="80"/>
+      <c r="E103" s="80"/>
+      <c r="F103" s="80"/>
+      <c r="G103" s="80"/>
+      <c r="H103" s="80"/>
+      <c r="I103" s="81"/>
     </row>
     <row r="105" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
@@ -6203,40 +6546,40 @@
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C168" s="3">
-        <v>1</v>
-      </c>
-      <c r="D168" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3"/>
-      <c r="H168" s="3"/>
+      <c r="A168" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="B168" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="C168" s="52">
+        <v>3</v>
+      </c>
+      <c r="D168" s="54"/>
+      <c r="E168" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="F168" s="54"/>
+      <c r="G168" s="54"/>
+      <c r="H168" s="54"/>
       <c r="I168" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
       <c r="C169" s="3">
         <v>1</v>
       </c>
-      <c r="D169" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E169" s="3"/>
+      <c r="D169" s="35"/>
+      <c r="E169" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
@@ -6244,20 +6587,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="B170" s="32" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="C170" s="3">
-        <v>1</v>
-      </c>
-      <c r="D170" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E170" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="D170" s="35"/>
+      <c r="E170" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
       <c r="H170" s="3"/>
@@ -6267,18 +6610,18 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="C171" s="3">
-        <v>5</v>
-      </c>
-      <c r="D171" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E171" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="D171" s="35"/>
+      <c r="E171" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="F171" s="3"/>
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
@@ -6288,18 +6631,18 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="C172" s="3">
-        <v>4</v>
-      </c>
-      <c r="D172" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E172" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="D172" s="35"/>
+      <c r="E172" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="F172" s="3"/>
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
@@ -6307,20 +6650,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>269</v>
+        <v>287</v>
+      </c>
+      <c r="B173" s="32" t="s">
+        <v>288</v>
       </c>
       <c r="C173" s="3">
-        <v>5</v>
-      </c>
-      <c r="D173" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E173" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="D173" s="35"/>
+      <c r="E173" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
@@ -6330,13 +6673,13 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>270</v>
+        <v>84</v>
       </c>
       <c r="C174" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D174" s="35" t="s">
         <v>80</v>
@@ -6351,10 +6694,10 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C175" s="3">
         <v>1</v>
@@ -6367,15 +6710,15 @@
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
       <c r="I175" s="20" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>85</v>
+        <v>257</v>
+      </c>
+      <c r="B176" s="32" t="s">
+        <v>268</v>
       </c>
       <c r="C176" s="3">
         <v>1</v>
@@ -6388,18 +6731,18 @@
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
       <c r="I176" s="20" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B177" s="32" t="s">
-        <v>268</v>
+        <v>258</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>263</v>
       </c>
       <c r="C177" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D177" s="35" t="s">
         <v>80</v>
@@ -6409,18 +6752,18 @@
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
       <c r="I177" s="20" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C178" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D178" s="35" t="s">
         <v>80</v>
@@ -6430,18 +6773,18 @@
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
       <c r="I178" s="20" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C179" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D179" s="35" t="s">
         <v>80</v>
@@ -6451,18 +6794,18 @@
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
       <c r="I179" s="20" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C180" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D180" s="35" t="s">
         <v>80</v>
@@ -6472,18 +6815,18 @@
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
       <c r="I180" s="20" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>270</v>
+        <v>84</v>
       </c>
       <c r="C181" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D181" s="35" t="s">
         <v>80</v>
@@ -6497,580 +6840,926 @@
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" s="3"/>
-      <c r="B182" s="3"/>
-      <c r="C182" s="3"/>
-      <c r="D182" s="3"/>
+      <c r="A182" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C182" s="3">
+        <v>1</v>
+      </c>
+      <c r="D182" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
-      <c r="I182" s="20"/>
+      <c r="I182" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="3"/>
-      <c r="B183" s="3"/>
-      <c r="C183" s="3"/>
-      <c r="D183" s="3"/>
+      <c r="A183" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B183" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C183" s="3">
+        <v>1</v>
+      </c>
+      <c r="D183" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="E183" s="3"/>
       <c r="F183" s="3"/>
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
-      <c r="I183" s="20"/>
+      <c r="I183" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="3"/>
-      <c r="B184" s="3"/>
-      <c r="C184" s="3"/>
-      <c r="D184" s="3"/>
+      <c r="A184" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C184" s="3">
+        <v>6</v>
+      </c>
+      <c r="D184" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="E184" s="3"/>
       <c r="F184" s="3"/>
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
-      <c r="I184" s="20"/>
+      <c r="I184" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="3"/>
-      <c r="B185" s="3"/>
-      <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
+      <c r="A185" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C185" s="3">
+        <v>3</v>
+      </c>
+      <c r="D185" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="E185" s="3"/>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
-      <c r="I185" s="20"/>
+      <c r="I185" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="3"/>
-      <c r="B186" s="3"/>
-      <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
+      <c r="A186" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C186" s="3">
+        <v>5</v>
+      </c>
+      <c r="D186" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="E186" s="3"/>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
-      <c r="I186" s="20"/>
+      <c r="I186" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="3"/>
-      <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
+      <c r="A187" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C187" s="3">
+        <v>3</v>
+      </c>
+      <c r="D187" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
       <c r="H187" s="3"/>
-      <c r="I187" s="20"/>
+      <c r="I187" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" s="3"/>
-      <c r="B188" s="3"/>
-      <c r="C188" s="3"/>
+      <c r="A188" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C188" s="3">
+        <v>1</v>
+      </c>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
-      <c r="F188" s="3"/>
+      <c r="F188" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
-      <c r="I188" s="20"/>
+      <c r="I188" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="3"/>
-      <c r="B189" s="3"/>
-      <c r="C189" s="3"/>
+      <c r="A189" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C189" s="3">
+        <v>5</v>
+      </c>
       <c r="D189" s="3"/>
       <c r="E189" s="3"/>
-      <c r="F189" s="3"/>
+      <c r="F189" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
-      <c r="I189" s="20"/>
+      <c r="I189" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="3"/>
-      <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
+      <c r="A190" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B190" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C190" s="3">
+        <v>2</v>
+      </c>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
-      <c r="F190" s="3"/>
+      <c r="F190" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
-      <c r="I190" s="20"/>
+      <c r="I190" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A191" s="3"/>
-      <c r="B191" s="3"/>
-      <c r="C191" s="3"/>
+      <c r="A191" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C191" s="3">
+        <v>6</v>
+      </c>
       <c r="D191" s="3"/>
       <c r="E191" s="3"/>
-      <c r="F191" s="3"/>
+      <c r="F191" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G191" s="3"/>
       <c r="H191" s="3"/>
-      <c r="I191" s="20"/>
+      <c r="I191" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" s="3"/>
-      <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
+      <c r="A192" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C192" s="3">
+        <v>6</v>
+      </c>
       <c r="D192" s="3"/>
       <c r="E192" s="3"/>
-      <c r="F192" s="3"/>
+      <c r="F192" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G192" s="3"/>
       <c r="H192" s="3"/>
-      <c r="I192" s="20"/>
+      <c r="I192" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="3"/>
-      <c r="B193" s="3"/>
-      <c r="C193" s="3"/>
+      <c r="A193" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C193" s="3">
+        <v>6</v>
+      </c>
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
-      <c r="F193" s="3"/>
+      <c r="F193" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G193" s="3"/>
       <c r="H193" s="3"/>
-      <c r="I193" s="20"/>
+      <c r="I193" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="3"/>
-      <c r="B194" s="3"/>
-      <c r="C194" s="3"/>
+      <c r="A194" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C194" s="3">
+        <v>6</v>
+      </c>
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
-      <c r="F194" s="3"/>
+      <c r="F194" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G194" s="3"/>
       <c r="H194" s="3"/>
-      <c r="I194" s="20"/>
+      <c r="I194" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" s="3"/>
-      <c r="B195" s="3"/>
-      <c r="C195" s="3"/>
-      <c r="D195" s="3"/>
-      <c r="E195" s="3"/>
-      <c r="F195" s="3"/>
-      <c r="G195" s="3"/>
-      <c r="H195" s="3"/>
-      <c r="I195" s="20"/>
+      <c r="A195" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C195" s="3">
+        <v>1</v>
+      </c>
+      <c r="D195" s="35"/>
+      <c r="E195" s="35"/>
+      <c r="F195" s="35"/>
+      <c r="G195" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H195" s="35"/>
+      <c r="I195" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A196" s="3"/>
-      <c r="B196" s="3"/>
-      <c r="C196" s="3"/>
-      <c r="D196" s="3"/>
-      <c r="E196" s="3"/>
-      <c r="F196" s="3"/>
-      <c r="G196" s="3"/>
-      <c r="H196" s="3"/>
-      <c r="I196" s="20"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A197" s="3"/>
-      <c r="B197" s="3"/>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
-      <c r="E197" s="3"/>
-      <c r="F197" s="3"/>
-      <c r="G197" s="3"/>
-      <c r="H197" s="3"/>
-      <c r="I197" s="20"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A198" s="3"/>
-      <c r="B198" s="3"/>
+      <c r="A196" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C196" s="3">
+        <v>2</v>
+      </c>
+      <c r="D196" s="35"/>
+      <c r="E196" s="35"/>
+      <c r="F196" s="35"/>
+      <c r="G196" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H196" s="35"/>
+      <c r="I196" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B197" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C197" s="3">
+        <v>2</v>
+      </c>
+      <c r="D197" s="35"/>
+      <c r="E197" s="35"/>
+      <c r="F197" s="35"/>
+      <c r="G197" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H197" s="35"/>
+      <c r="I197" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B198" s="32" t="s">
+        <v>308</v>
+      </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
       <c r="E198" s="3"/>
       <c r="F198" s="3"/>
-      <c r="G198" s="3"/>
+      <c r="G198" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H198" s="3"/>
-      <c r="I198" s="20"/>
+      <c r="I198" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" s="3"/>
-      <c r="B199" s="3"/>
-      <c r="C199" s="3"/>
+      <c r="A199" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C199" s="3">
+        <v>5</v>
+      </c>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
       <c r="F199" s="3"/>
-      <c r="G199" s="3"/>
+      <c r="G199" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H199" s="3"/>
-      <c r="I199" s="20"/>
+      <c r="I199" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" s="3"/>
-      <c r="B200" s="3"/>
-      <c r="C200" s="3"/>
+      <c r="A200" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C200" s="3">
+        <v>1</v>
+      </c>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
       <c r="F200" s="3"/>
-      <c r="G200" s="3"/>
+      <c r="G200" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H200" s="3"/>
-      <c r="I200" s="20"/>
+      <c r="I200" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A201" s="3"/>
-      <c r="B201" s="3"/>
-      <c r="C201" s="3"/>
+      <c r="A201" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C201" s="3">
+        <v>4</v>
+      </c>
       <c r="D201" s="3"/>
       <c r="E201" s="3"/>
       <c r="F201" s="3"/>
-      <c r="G201" s="3"/>
+      <c r="G201" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H201" s="3"/>
-      <c r="I201" s="20"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A202" s="3"/>
-      <c r="B202" s="3"/>
-      <c r="C202" s="3"/>
+      <c r="I201" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B202" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C202" s="3">
+        <v>1</v>
+      </c>
       <c r="D202" s="3"/>
       <c r="E202" s="3"/>
       <c r="F202" s="3"/>
-      <c r="G202" s="3"/>
+      <c r="G202" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H202" s="3"/>
-      <c r="I202" s="20"/>
+      <c r="I202" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A203" s="3"/>
-      <c r="B203" s="3"/>
+      <c r="A203" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B203" s="32" t="s">
+        <v>306</v>
+      </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
       <c r="E203" s="3"/>
       <c r="F203" s="3"/>
-      <c r="G203" s="3"/>
+      <c r="G203" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H203" s="3"/>
-      <c r="I203" s="20"/>
+      <c r="I203" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A204" s="3"/>
-      <c r="B204" s="3"/>
-      <c r="C204" s="3"/>
+      <c r="A204" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C204" s="3">
+        <v>8</v>
+      </c>
       <c r="D204" s="3"/>
       <c r="E204" s="3"/>
       <c r="F204" s="3"/>
-      <c r="G204" s="3"/>
+      <c r="G204" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H204" s="3"/>
-      <c r="I204" s="20"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A205" s="3"/>
-      <c r="B205" s="3"/>
-      <c r="C205" s="3"/>
+      <c r="I204" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B205" s="82" t="s">
+        <v>311</v>
+      </c>
+      <c r="C205" s="3">
+        <v>8</v>
+      </c>
       <c r="D205" s="3"/>
       <c r="E205" s="3"/>
       <c r="F205" s="3"/>
-      <c r="G205" s="3"/>
+      <c r="G205" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H205" s="3"/>
-      <c r="I205" s="20"/>
+      <c r="I205" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A206" s="3"/>
-      <c r="B206" s="3"/>
-      <c r="C206" s="3"/>
+      <c r="A206" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C206" s="3">
+        <v>8</v>
+      </c>
       <c r="D206" s="3"/>
       <c r="E206" s="3"/>
       <c r="F206" s="3"/>
-      <c r="G206" s="3"/>
+      <c r="G206" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="H206" s="3"/>
-      <c r="I206" s="20"/>
+      <c r="I206" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A207" s="3"/>
-      <c r="B207" s="3"/>
-      <c r="C207" s="3"/>
+      <c r="A207" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B207" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="C207" s="3">
+        <v>2</v>
+      </c>
       <c r="D207" s="3"/>
       <c r="E207" s="3"/>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
-      <c r="H207" s="3"/>
-      <c r="I207" s="20"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A208" s="3"/>
-      <c r="B208" s="3"/>
-      <c r="C208" s="3"/>
+      <c r="H207" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I207" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B208" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="C208" s="3">
+        <v>3</v>
+      </c>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
-      <c r="H208" s="3"/>
-      <c r="I208" s="20"/>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A209" s="3"/>
-      <c r="B209" s="3"/>
-      <c r="C209" s="3"/>
+      <c r="H208" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I208" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B209" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="C209" s="3">
+        <v>4</v>
+      </c>
       <c r="D209" s="3"/>
       <c r="E209" s="3"/>
       <c r="F209" s="3"/>
       <c r="G209" s="3"/>
-      <c r="H209" s="3"/>
-      <c r="I209" s="20"/>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A210" s="3"/>
-      <c r="B210" s="3"/>
-      <c r="C210" s="3"/>
+      <c r="H209" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I209" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B210" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="C210" s="3">
+        <v>5</v>
+      </c>
       <c r="D210" s="3"/>
       <c r="E210" s="3"/>
       <c r="F210" s="3"/>
       <c r="G210" s="3"/>
-      <c r="H210" s="3"/>
-      <c r="I210" s="20"/>
+      <c r="H210" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I210" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A211" s="3"/>
-      <c r="B211" s="3"/>
-      <c r="C211" s="3"/>
+      <c r="A211" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B211" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="C211" s="3">
+        <v>7</v>
+      </c>
       <c r="D211" s="3"/>
       <c r="E211" s="3"/>
       <c r="F211" s="3"/>
       <c r="G211" s="3"/>
-      <c r="H211" s="3"/>
-      <c r="I211" s="20"/>
+      <c r="H211" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I211" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A212" s="3"/>
-      <c r="B212" s="3"/>
-      <c r="C212" s="3"/>
+      <c r="A212" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B212" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="C212" s="3">
+        <v>7</v>
+      </c>
       <c r="D212" s="3"/>
       <c r="E212" s="3"/>
       <c r="F212" s="3"/>
       <c r="G212" s="3"/>
-      <c r="H212" s="3"/>
-      <c r="I212" s="20"/>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A213" s="3"/>
-      <c r="B213" s="3"/>
-      <c r="C213" s="3"/>
+      <c r="H212" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I212" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B213" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="C213" s="3">
+        <v>6</v>
+      </c>
       <c r="D213" s="3"/>
       <c r="E213" s="3"/>
       <c r="F213" s="3"/>
       <c r="G213" s="3"/>
-      <c r="H213" s="3"/>
-      <c r="I213" s="20"/>
+      <c r="H213" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I213" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A214" s="3"/>
-      <c r="B214" s="3"/>
-      <c r="C214" s="3"/>
+      <c r="A214" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B214" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="C214" s="3">
+        <v>5</v>
+      </c>
       <c r="D214" s="3"/>
       <c r="E214" s="3"/>
       <c r="F214" s="3"/>
       <c r="G214" s="3"/>
-      <c r="H214" s="3"/>
-      <c r="I214" s="20"/>
-    </row>
-    <row r="215" spans="1:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="24"/>
-      <c r="B215" s="25"/>
-      <c r="C215" s="25"/>
-      <c r="D215" s="25"/>
-      <c r="E215" s="25"/>
-      <c r="F215" s="25"/>
-      <c r="G215" s="25"/>
-      <c r="H215" s="25"/>
-      <c r="I215" s="21" t="s">
-        <v>32</v>
+      <c r="H214" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I214" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B215" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="C215" s="3">
+        <v>2</v>
+      </c>
+      <c r="D215" s="3"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="3"/>
+      <c r="G215" s="3"/>
+      <c r="H215" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I215" s="20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A216" s="18"/>
-      <c r="B216" s="23"/>
-      <c r="C216" s="23"/>
-      <c r="D216" s="23"/>
-      <c r="E216" s="23"/>
-      <c r="F216" s="23"/>
-      <c r="G216" s="23"/>
-      <c r="H216" s="23"/>
-      <c r="I216" s="19" t="s">
+      <c r="A216" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B216" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="C216" s="3">
+        <v>2</v>
+      </c>
+      <c r="D216" s="3"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
+      <c r="H216" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I216" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A217" s="26"/>
-      <c r="B217" s="27"/>
-      <c r="C217" s="27"/>
-      <c r="D217" s="27"/>
-      <c r="E217" s="27"/>
-      <c r="F217" s="27"/>
-      <c r="G217" s="27"/>
-      <c r="H217" s="27"/>
-      <c r="I217" s="22" t="s">
+      <c r="A217" s="3"/>
+      <c r="B217" s="3"/>
+      <c r="C217" s="3"/>
+      <c r="D217" s="3"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="3"/>
+      <c r="G217" s="3"/>
+      <c r="H217" s="35"/>
+      <c r="I217" s="20"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218" s="3"/>
+      <c r="B218" s="3"/>
+      <c r="C218" s="3"/>
+      <c r="D218" s="3"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="3"/>
+      <c r="G218" s="3"/>
+      <c r="H218" s="35"/>
+      <c r="I218" s="20"/>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A219" s="3"/>
+      <c r="B219" s="3"/>
+      <c r="C219" s="3"/>
+      <c r="D219" s="3"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
+      <c r="H219" s="3"/>
+      <c r="I219" s="20"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A220" s="3"/>
+      <c r="B220" s="3"/>
+      <c r="C220" s="3"/>
+      <c r="D220" s="3"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+      <c r="H220" s="3"/>
+      <c r="I220" s="20"/>
+    </row>
+    <row r="221" spans="1:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="24"/>
+      <c r="B221" s="25"/>
+      <c r="C221" s="25"/>
+      <c r="D221" s="25"/>
+      <c r="E221" s="25"/>
+      <c r="F221" s="25"/>
+      <c r="G221" s="25"/>
+      <c r="H221" s="25"/>
+      <c r="I221" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A222" s="18"/>
+      <c r="B222" s="23"/>
+      <c r="C222" s="23"/>
+      <c r="D222" s="23"/>
+      <c r="E222" s="23"/>
+      <c r="F222" s="23"/>
+      <c r="G222" s="23"/>
+      <c r="H222" s="23"/>
+      <c r="I222" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223" s="26"/>
+      <c r="B223" s="27"/>
+      <c r="C223" s="27"/>
+      <c r="D223" s="27"/>
+      <c r="E223" s="27"/>
+      <c r="F223" s="27"/>
+      <c r="G223" s="27"/>
+      <c r="H223" s="27"/>
+      <c r="I223" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A218" s="39" t="s">
+    <row r="224" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A224" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B218" s="40"/>
-      <c r="C218" s="40"/>
-      <c r="D218" s="40"/>
-      <c r="E218" s="40"/>
-      <c r="F218" s="40"/>
-      <c r="G218" s="40"/>
-      <c r="H218" s="40"/>
-      <c r="I218" s="41"/>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A219" s="42"/>
-      <c r="B219" s="43"/>
-      <c r="C219" s="43"/>
-      <c r="D219" s="43"/>
-      <c r="E219" s="43"/>
-      <c r="F219" s="43"/>
-      <c r="G219" s="43"/>
-      <c r="H219" s="43"/>
-      <c r="I219" s="44"/>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A220" s="45"/>
-      <c r="B220" s="46"/>
-      <c r="C220" s="46"/>
-      <c r="D220" s="46"/>
-      <c r="E220" s="46"/>
-      <c r="F220" s="46"/>
-      <c r="G220" s="46"/>
-      <c r="H220" s="46"/>
-      <c r="I220" s="47"/>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A221" s="45"/>
-      <c r="B221" s="46"/>
-      <c r="C221" s="46"/>
-      <c r="D221" s="46"/>
-      <c r="E221" s="46"/>
-      <c r="F221" s="46"/>
-      <c r="G221" s="46"/>
-      <c r="H221" s="46"/>
-      <c r="I221" s="47"/>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A222" s="45"/>
-      <c r="B222" s="46"/>
-      <c r="C222" s="46"/>
-      <c r="D222" s="46"/>
-      <c r="E222" s="46"/>
-      <c r="F222" s="46"/>
-      <c r="G222" s="46"/>
-      <c r="H222" s="46"/>
-      <c r="I222" s="47"/>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A223" s="48"/>
-      <c r="B223" s="49"/>
-      <c r="C223" s="49"/>
-      <c r="D223" s="49"/>
-      <c r="E223" s="49"/>
-      <c r="F223" s="49"/>
-      <c r="G223" s="49"/>
-      <c r="H223" s="49"/>
-      <c r="I223" s="50"/>
-    </row>
-    <row r="225" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A225" s="1" t="s">
+      <c r="B224" s="40"/>
+      <c r="C224" s="40"/>
+      <c r="D224" s="40"/>
+      <c r="E224" s="40"/>
+      <c r="F224" s="40"/>
+      <c r="G224" s="40"/>
+      <c r="H224" s="40"/>
+      <c r="I224" s="41"/>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A225" s="42"/>
+      <c r="B225" s="43"/>
+      <c r="C225" s="43"/>
+      <c r="D225" s="43"/>
+      <c r="E225" s="43"/>
+      <c r="F225" s="43"/>
+      <c r="G225" s="43"/>
+      <c r="H225" s="43"/>
+      <c r="I225" s="44"/>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A226" s="45"/>
+      <c r="B226" s="46"/>
+      <c r="C226" s="46"/>
+      <c r="D226" s="46"/>
+      <c r="E226" s="46"/>
+      <c r="F226" s="46"/>
+      <c r="G226" s="46"/>
+      <c r="H226" s="46"/>
+      <c r="I226" s="47"/>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A227" s="45"/>
+      <c r="B227" s="46"/>
+      <c r="C227" s="46"/>
+      <c r="D227" s="46"/>
+      <c r="E227" s="46"/>
+      <c r="F227" s="46"/>
+      <c r="G227" s="46"/>
+      <c r="H227" s="46"/>
+      <c r="I227" s="47"/>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A228" s="45"/>
+      <c r="B228" s="46"/>
+      <c r="C228" s="46"/>
+      <c r="D228" s="46"/>
+      <c r="E228" s="46"/>
+      <c r="F228" s="46"/>
+      <c r="G228" s="46"/>
+      <c r="H228" s="46"/>
+      <c r="I228" s="47"/>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229" s="48"/>
+      <c r="B229" s="49"/>
+      <c r="C229" s="49"/>
+      <c r="D229" s="49"/>
+      <c r="E229" s="49"/>
+      <c r="F229" s="49"/>
+      <c r="G229" s="49"/>
+      <c r="H229" s="49"/>
+      <c r="I229" s="50"/>
+    </row>
+    <row r="231" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A231" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A226" s="28" t="s">
+    <row r="232" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A232" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B226" s="29"/>
-    </row>
-    <row r="228" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A228" s="4" t="s">
+      <c r="B232" s="29"/>
+    </row>
+    <row r="234" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A234" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B228" s="4" t="s">
+      <c r="B234" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C228" s="4" t="s">
+      <c r="C234" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D228" s="12" t="s">
+      <c r="D234" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E228" s="12" t="s">
+      <c r="E234" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F228" s="12" t="s">
+      <c r="F234" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G228" s="12" t="s">
+      <c r="G234" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H228" s="12" t="s">
+      <c r="H234" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I228" s="4" t="s">
+      <c r="I234" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A229" s="3"/>
-      <c r="B229" s="3"/>
-      <c r="C229" s="3"/>
-      <c r="D229" s="3"/>
-      <c r="E229" s="3"/>
-      <c r="F229" s="3"/>
-      <c r="G229" s="3"/>
-      <c r="H229" s="3"/>
-      <c r="I229" s="20"/>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A230" s="3"/>
-      <c r="B230" s="3"/>
-      <c r="C230" s="3"/>
-      <c r="D230" s="3"/>
-      <c r="E230" s="3"/>
-      <c r="F230" s="3"/>
-      <c r="G230" s="3"/>
-      <c r="H230" s="3"/>
-      <c r="I230" s="20"/>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A231" s="3"/>
-      <c r="B231" s="3"/>
-      <c r="C231" s="3"/>
-      <c r="D231" s="3"/>
-      <c r="E231" s="3"/>
-      <c r="F231" s="3"/>
-      <c r="G231" s="3"/>
-      <c r="H231" s="3"/>
-      <c r="I231" s="20"/>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A232" s="3"/>
-      <c r="B232" s="3"/>
-      <c r="C232" s="3"/>
-      <c r="D232" s="3"/>
-      <c r="E232" s="3"/>
-      <c r="F232" s="3"/>
-      <c r="G232" s="3"/>
-      <c r="H232" s="3"/>
-      <c r="I232" s="20"/>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A233" s="3"/>
-      <c r="B233" s="3"/>
-      <c r="C233" s="3"/>
-      <c r="D233" s="3"/>
-      <c r="E233" s="3"/>
-      <c r="F233" s="3"/>
-      <c r="G233" s="3"/>
-      <c r="H233" s="3"/>
-      <c r="I233" s="20"/>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A234" s="3"/>
-      <c r="B234" s="3"/>
-      <c r="C234" s="3"/>
-      <c r="D234" s="3"/>
-      <c r="E234" s="3"/>
-      <c r="F234" s="3"/>
-      <c r="G234" s="3"/>
-      <c r="H234" s="3"/>
-      <c r="I234" s="20"/>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="3"/>
@@ -7491,111 +8180,177 @@
       <c r="I272" s="20"/>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A273" s="24"/>
-      <c r="B273" s="25"/>
-      <c r="C273" s="25"/>
-      <c r="D273" s="25"/>
-      <c r="E273" s="25"/>
-      <c r="F273" s="25"/>
-      <c r="G273" s="25"/>
-      <c r="H273" s="25"/>
-      <c r="I273" s="21" t="s">
-        <v>32</v>
-      </c>
+      <c r="A273" s="3"/>
+      <c r="B273" s="3"/>
+      <c r="C273" s="3"/>
+      <c r="D273" s="3"/>
+      <c r="E273" s="3"/>
+      <c r="F273" s="3"/>
+      <c r="G273" s="3"/>
+      <c r="H273" s="3"/>
+      <c r="I273" s="20"/>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A274" s="18"/>
-      <c r="B274" s="23"/>
-      <c r="C274" s="23"/>
-      <c r="D274" s="23"/>
-      <c r="E274" s="23"/>
-      <c r="F274" s="23"/>
-      <c r="G274" s="23"/>
-      <c r="H274" s="23"/>
-      <c r="I274" s="19" t="s">
+      <c r="A274" s="3"/>
+      <c r="B274" s="3"/>
+      <c r="C274" s="3"/>
+      <c r="D274" s="3"/>
+      <c r="E274" s="3"/>
+      <c r="F274" s="3"/>
+      <c r="G274" s="3"/>
+      <c r="H274" s="3"/>
+      <c r="I274" s="20"/>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A275" s="3"/>
+      <c r="B275" s="3"/>
+      <c r="C275" s="3"/>
+      <c r="D275" s="3"/>
+      <c r="E275" s="3"/>
+      <c r="F275" s="3"/>
+      <c r="G275" s="3"/>
+      <c r="H275" s="3"/>
+      <c r="I275" s="20"/>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A276" s="3"/>
+      <c r="B276" s="3"/>
+      <c r="C276" s="3"/>
+      <c r="D276" s="3"/>
+      <c r="E276" s="3"/>
+      <c r="F276" s="3"/>
+      <c r="G276" s="3"/>
+      <c r="H276" s="3"/>
+      <c r="I276" s="20"/>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A277" s="3"/>
+      <c r="B277" s="3"/>
+      <c r="C277" s="3"/>
+      <c r="D277" s="3"/>
+      <c r="E277" s="3"/>
+      <c r="F277" s="3"/>
+      <c r="G277" s="3"/>
+      <c r="H277" s="3"/>
+      <c r="I277" s="20"/>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A278" s="3"/>
+      <c r="B278" s="3"/>
+      <c r="C278" s="3"/>
+      <c r="D278" s="3"/>
+      <c r="E278" s="3"/>
+      <c r="F278" s="3"/>
+      <c r="G278" s="3"/>
+      <c r="H278" s="3"/>
+      <c r="I278" s="20"/>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A279" s="24"/>
+      <c r="B279" s="25"/>
+      <c r="C279" s="25"/>
+      <c r="D279" s="25"/>
+      <c r="E279" s="25"/>
+      <c r="F279" s="25"/>
+      <c r="G279" s="25"/>
+      <c r="H279" s="25"/>
+      <c r="I279" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A280" s="18"/>
+      <c r="B280" s="23"/>
+      <c r="C280" s="23"/>
+      <c r="D280" s="23"/>
+      <c r="E280" s="23"/>
+      <c r="F280" s="23"/>
+      <c r="G280" s="23"/>
+      <c r="H280" s="23"/>
+      <c r="I280" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A275" s="26"/>
-      <c r="B275" s="27"/>
-      <c r="C275" s="27"/>
-      <c r="D275" s="27"/>
-      <c r="E275" s="27"/>
-      <c r="F275" s="27"/>
-      <c r="G275" s="27"/>
-      <c r="H275" s="27"/>
-      <c r="I275" s="22" t="s">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A281" s="26"/>
+      <c r="B281" s="27"/>
+      <c r="C281" s="27"/>
+      <c r="D281" s="27"/>
+      <c r="E281" s="27"/>
+      <c r="F281" s="27"/>
+      <c r="G281" s="27"/>
+      <c r="H281" s="27"/>
+      <c r="I281" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="276" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A276" s="39" t="s">
+    <row r="282" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A282" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B276" s="40"/>
-      <c r="C276" s="40"/>
-      <c r="D276" s="40"/>
-      <c r="E276" s="40"/>
-      <c r="F276" s="40"/>
-      <c r="G276" s="40"/>
-      <c r="H276" s="40"/>
-      <c r="I276" s="41"/>
-    </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A277" s="42"/>
-      <c r="B277" s="43"/>
-      <c r="C277" s="43"/>
-      <c r="D277" s="43"/>
-      <c r="E277" s="43"/>
-      <c r="F277" s="43"/>
-      <c r="G277" s="43"/>
-      <c r="H277" s="43"/>
-      <c r="I277" s="44"/>
-    </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A278" s="45"/>
-      <c r="B278" s="46"/>
-      <c r="C278" s="46"/>
-      <c r="D278" s="46"/>
-      <c r="E278" s="46"/>
-      <c r="F278" s="46"/>
-      <c r="G278" s="46"/>
-      <c r="H278" s="46"/>
-      <c r="I278" s="47"/>
-    </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A279" s="45"/>
-      <c r="B279" s="46"/>
-      <c r="C279" s="46"/>
-      <c r="D279" s="46"/>
-      <c r="E279" s="46"/>
-      <c r="F279" s="46"/>
-      <c r="G279" s="46"/>
-      <c r="H279" s="46"/>
-      <c r="I279" s="47"/>
-    </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A280" s="45"/>
-      <c r="B280" s="46"/>
-      <c r="C280" s="46"/>
-      <c r="D280" s="46"/>
-      <c r="E280" s="46"/>
-      <c r="F280" s="46"/>
-      <c r="G280" s="46"/>
-      <c r="H280" s="46"/>
-      <c r="I280" s="47"/>
-    </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A281" s="48"/>
-      <c r="B281" s="49"/>
-      <c r="C281" s="49"/>
-      <c r="D281" s="49"/>
-      <c r="E281" s="49"/>
-      <c r="F281" s="49"/>
-      <c r="G281" s="49"/>
-      <c r="H281" s="49"/>
-      <c r="I281" s="50"/>
+      <c r="B282" s="40"/>
+      <c r="C282" s="40"/>
+      <c r="D282" s="40"/>
+      <c r="E282" s="40"/>
+      <c r="F282" s="40"/>
+      <c r="G282" s="40"/>
+      <c r="H282" s="40"/>
+      <c r="I282" s="41"/>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A283" s="42"/>
+      <c r="B283" s="43"/>
+      <c r="C283" s="43"/>
+      <c r="D283" s="43"/>
+      <c r="E283" s="43"/>
+      <c r="F283" s="43"/>
+      <c r="G283" s="43"/>
+      <c r="H283" s="43"/>
+      <c r="I283" s="44"/>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A284" s="45"/>
+      <c r="B284" s="46"/>
+      <c r="C284" s="46"/>
+      <c r="D284" s="46"/>
+      <c r="E284" s="46"/>
+      <c r="F284" s="46"/>
+      <c r="G284" s="46"/>
+      <c r="H284" s="46"/>
+      <c r="I284" s="47"/>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A285" s="45"/>
+      <c r="B285" s="46"/>
+      <c r="C285" s="46"/>
+      <c r="D285" s="46"/>
+      <c r="E285" s="46"/>
+      <c r="F285" s="46"/>
+      <c r="G285" s="46"/>
+      <c r="H285" s="46"/>
+      <c r="I285" s="47"/>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A286" s="45"/>
+      <c r="B286" s="46"/>
+      <c r="C286" s="46"/>
+      <c r="D286" s="46"/>
+      <c r="E286" s="46"/>
+      <c r="F286" s="46"/>
+      <c r="G286" s="46"/>
+      <c r="H286" s="46"/>
+      <c r="I286" s="47"/>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A287" s="48"/>
+      <c r="B287" s="49"/>
+      <c r="C287" s="49"/>
+      <c r="D287" s="49"/>
+      <c r="E287" s="49"/>
+      <c r="F287" s="49"/>
+      <c r="G287" s="49"/>
+      <c r="H287" s="49"/>
+      <c r="I287" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7604,7 +8359,7 @@
     <mergeCell ref="A99:I103"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I229:I272 I12:I94 I109:I156 I168:I214">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I235:I278 I12:I94 I109:I156 I168:I220">
       <formula1>$I$95:$I$97</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>